<commit_message>
delete obscure comment text
</commit_message>
<xml_diff>
--- a/support/sample.xlsx
+++ b/support/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="23580" windowHeight="11250" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="23580" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
   <si>
     <t>行</t>
     <rPh sb="0" eb="1">
@@ -32,19 +32,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>7833分≒5日で解けた</t>
-    <rPh sb="4" eb="5">
-      <t>フン</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ニチ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>短絡</t>
     <rPh sb="0" eb="2">
       <t>タンラク</t>
@@ -52,23 +39,14 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>NL_sample00.xls sheet3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NL_sample00.xls sheet12</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1時間ではとけない</t>
-    <rPh sb="1" eb="3">
-      <t>ジカン</t>
+    <t>解は1つだけだと思う</t>
+    <rPh sb="0" eb="1">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>オモ</t>
     </rPh>
     <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>NL_sample00.xls sheet4</t>
-    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -538,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1574,7 +1552,7 @@
         <v>16</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.15">
@@ -1595,9 +1573,6 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>20</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.15">
@@ -2946,7 +2921,7 @@
         <v>20</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.15">
@@ -2957,9 +2932,6 @@
     <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>22</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.15">
@@ -3038,8 +3010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4298,7 +4270,7 @@
         <v>20</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.15">
@@ -4314,9 +4286,6 @@
     <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>23</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add ADC2016 rule(multi-layer) support
</commit_message>
<xml_diff>
--- a/support/sample.xlsx
+++ b/support/sample.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="23580" windowHeight="11250"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="23580" windowHeight="11250" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="1" r:id="rId1"/>
     <sheet name="Q2" sheetId="2" r:id="rId2"/>
     <sheet name="Q3" sheetId="3" r:id="rId3"/>
+    <sheet name="Q4.1" sheetId="4" r:id="rId4"/>
+    <sheet name="Q4.2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>行</t>
     <rPh sb="0" eb="1">
@@ -47,6 +49,94 @@
       <t>オモ</t>
     </rPh>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>c=1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>b=2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>d=3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>a=4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>e=5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>層</t>
+    <rPh sb="0" eb="1">
+      <t>ソウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>使用した数字</t>
+    <rPh sb="0" eb="2">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>スウジ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>使用したアルファベット</t>
+    <rPh sb="0" eb="2">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>a,b,c,d,e</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>他の層で使用した数字</t>
+    <rPh sb="0" eb="1">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ソウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>スウジ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>6,7</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,   8,9,10</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8,9,10</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -92,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,13 +266,115 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -194,7 +386,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -212,6 +404,17 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="アクセント 1" xfId="1" builtinId="29"/>
@@ -516,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -525,19 +728,20 @@
     <col min="1" max="16384" width="3.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="A1" s="1">
+    <row r="1" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1662,7 +1866,7 @@
   <dimension ref="A1:AK39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1670,19 +1874,20 @@
     <col min="1" max="16384" width="3.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="A1" s="1">
+    <row r="1" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3011,7 +3216,7 @@
   <dimension ref="A1:AK39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3019,19 +3224,22 @@
     <col min="1" max="16384" width="3.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="A1" s="1">
+    <row r="1" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
+      <c r="C1" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4309,6 +4517,1960 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A32" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="2">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="16384" width="3.5" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19">
+        <v>10</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="21">
+        <v>1</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22">
+        <v>2</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20">
+        <v>10</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2">
+        <v>9</v>
+      </c>
+      <c r="L3" s="2">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2">
+        <v>12</v>
+      </c>
+      <c r="O3" s="2">
+        <v>13</v>
+      </c>
+      <c r="P3" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>15</v>
+      </c>
+      <c r="R3" s="2">
+        <v>16</v>
+      </c>
+      <c r="S3" s="2">
+        <v>17</v>
+      </c>
+      <c r="T3" s="2">
+        <v>18</v>
+      </c>
+      <c r="U3" s="2">
+        <v>19</v>
+      </c>
+      <c r="V3" s="2">
+        <v>20</v>
+      </c>
+      <c r="W3" s="2">
+        <v>21</v>
+      </c>
+      <c r="X3" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>25</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>27</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>29</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>30</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>31</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>32</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>33</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>34</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11">
+        <v>2</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2</v>
+      </c>
+      <c r="F4" s="11">
+        <v>2</v>
+      </c>
+      <c r="G4" s="11">
+        <v>2</v>
+      </c>
+      <c r="H4" s="11">
+        <v>2</v>
+      </c>
+      <c r="I4" s="11">
+        <v>2</v>
+      </c>
+      <c r="J4" s="11">
+        <v>2</v>
+      </c>
+      <c r="K4" s="11">
+        <v>2</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="11">
+        <v>2</v>
+      </c>
+      <c r="C5" s="12">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>5</v>
+      </c>
+      <c r="E5" s="12">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12">
+        <v>5</v>
+      </c>
+      <c r="G5" s="12">
+        <v>5</v>
+      </c>
+      <c r="H5" s="12">
+        <v>5</v>
+      </c>
+      <c r="I5" s="12">
+        <v>5</v>
+      </c>
+      <c r="J5" s="12">
+        <v>5</v>
+      </c>
+      <c r="K5" s="11">
+        <v>2</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>5</v>
+      </c>
+      <c r="D6" s="9">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9">
+        <v>4</v>
+      </c>
+      <c r="F6" s="9">
+        <v>4</v>
+      </c>
+      <c r="G6" s="9">
+        <v>4</v>
+      </c>
+      <c r="H6" s="9">
+        <v>4</v>
+      </c>
+      <c r="I6" s="9">
+        <v>4</v>
+      </c>
+      <c r="J6" s="12">
+        <v>5</v>
+      </c>
+      <c r="K6" s="11">
+        <v>2</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="11">
+        <v>2</v>
+      </c>
+      <c r="C7" s="12">
+        <v>5</v>
+      </c>
+      <c r="D7" s="9">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
+        <v>2</v>
+      </c>
+      <c r="I7" s="12">
+        <v>5</v>
+      </c>
+      <c r="J7" s="12">
+        <v>5</v>
+      </c>
+      <c r="K7" s="11">
+        <v>2</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="11">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12">
+        <v>5</v>
+      </c>
+      <c r="D8" s="9">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="12">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11">
+        <v>2</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="11">
+        <v>2</v>
+      </c>
+      <c r="K8" s="11">
+        <v>2</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2</v>
+      </c>
+      <c r="C9" s="12">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12">
+        <v>5</v>
+      </c>
+      <c r="E9" s="12">
+        <v>5</v>
+      </c>
+      <c r="F9" s="12">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <v>2</v>
+      </c>
+      <c r="I9" s="11">
+        <v>2</v>
+      </c>
+      <c r="J9" s="11">
+        <v>2</v>
+      </c>
+      <c r="K9" s="8">
+        <v>9</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2</v>
+      </c>
+      <c r="E10" s="11">
+        <v>2</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="8">
+        <v>9</v>
+      </c>
+      <c r="J10" s="5">
+        <v>10</v>
+      </c>
+      <c r="K10" s="8">
+        <v>9</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3</v>
+      </c>
+      <c r="E11" s="6">
+        <v>3</v>
+      </c>
+      <c r="F11" s="6">
+        <v>3</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>3</v>
+      </c>
+      <c r="I11" s="8">
+        <v>9</v>
+      </c>
+      <c r="J11" s="5">
+        <v>10</v>
+      </c>
+      <c r="K11" s="8">
+        <v>9</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4">
+        <v>8</v>
+      </c>
+      <c r="F12" s="4">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="6">
+        <v>3</v>
+      </c>
+      <c r="I12" s="8">
+        <v>9</v>
+      </c>
+      <c r="J12" s="5">
+        <v>10</v>
+      </c>
+      <c r="K12" s="8">
+        <v>9</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6">
+        <v>3</v>
+      </c>
+      <c r="H13" s="6">
+        <v>3</v>
+      </c>
+      <c r="I13" s="8">
+        <v>9</v>
+      </c>
+      <c r="J13" s="8">
+        <v>9</v>
+      </c>
+      <c r="K13" s="8">
+        <v>9</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A15" s="2">
+        <v>11</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A16" s="2">
+        <v>12</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A20" s="2">
+        <v>16</v>
+      </c>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A22" s="2">
+        <v>18</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A23" s="2">
+        <v>19</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A24" s="2">
+        <v>20</v>
+      </c>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A25" s="2">
+        <v>21</v>
+      </c>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A26" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A27" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A28" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A29" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A30" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A31" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A32" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="2">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="16384" width="3.5" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19">
+        <v>10</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="21">
+        <v>2</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22">
+        <v>2</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20">
+        <v>10</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2">
+        <v>9</v>
+      </c>
+      <c r="L3" s="2">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2">
+        <v>12</v>
+      </c>
+      <c r="O3" s="2">
+        <v>13</v>
+      </c>
+      <c r="P3" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>15</v>
+      </c>
+      <c r="R3" s="2">
+        <v>16</v>
+      </c>
+      <c r="S3" s="2">
+        <v>17</v>
+      </c>
+      <c r="T3" s="2">
+        <v>18</v>
+      </c>
+      <c r="U3" s="2">
+        <v>19</v>
+      </c>
+      <c r="V3" s="2">
+        <v>20</v>
+      </c>
+      <c r="W3" s="2">
+        <v>21</v>
+      </c>
+      <c r="X3" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>25</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>27</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>29</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>30</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>31</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>32</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>33</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>34</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="11">
+        <v>2</v>
+      </c>
+      <c r="G4" s="11">
+        <v>2</v>
+      </c>
+      <c r="H4" s="11">
+        <v>2</v>
+      </c>
+      <c r="I4" s="11">
+        <v>2</v>
+      </c>
+      <c r="J4" s="11">
+        <v>2</v>
+      </c>
+      <c r="K4" s="11">
+        <v>2</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>4</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4</v>
+      </c>
+      <c r="E5" s="9">
+        <v>4</v>
+      </c>
+      <c r="F5" s="11">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="11">
+        <v>2</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4</v>
+      </c>
+      <c r="D6" s="14">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9">
+        <v>4</v>
+      </c>
+      <c r="F6" s="11">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <v>5</v>
+      </c>
+      <c r="I6" s="12">
+        <v>5</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
+      <c r="K6" s="11">
+        <v>2</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6">
+        <v>3</v>
+      </c>
+      <c r="C7" s="9">
+        <v>4</v>
+      </c>
+      <c r="D7" s="14">
+        <v>7</v>
+      </c>
+      <c r="E7" s="9">
+        <v>4</v>
+      </c>
+      <c r="F7" s="11">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
+        <v>2</v>
+      </c>
+      <c r="I7" s="12">
+        <v>5</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="11">
+        <v>2</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9">
+        <v>4</v>
+      </c>
+      <c r="D8" s="14">
+        <v>7</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="11">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11">
+        <v>2</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+      <c r="K8" s="11">
+        <v>2</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="14">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4">
+        <v>6</v>
+      </c>
+      <c r="F9" s="11">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <v>2</v>
+      </c>
+      <c r="I9" s="11">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" s="11">
+        <v>2</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9">
+        <v>4</v>
+      </c>
+      <c r="D10" s="14">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4">
+        <v>6</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="11">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="11">
+        <v>2</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9">
+        <v>4</v>
+      </c>
+      <c r="D11" s="14">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4">
+        <v>6</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>3</v>
+      </c>
+      <c r="I11" s="11">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
+      <c r="K11" s="11">
+        <v>2</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6">
+        <v>3</v>
+      </c>
+      <c r="C12" s="9">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9">
+        <v>4</v>
+      </c>
+      <c r="F12" s="9">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="6">
+        <v>3</v>
+      </c>
+      <c r="I12" s="11">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+      <c r="K12" s="11">
+        <v>2</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6">
+        <v>3</v>
+      </c>
+      <c r="H13" s="6">
+        <v>3</v>
+      </c>
+      <c r="I13" s="11">
+        <v>2</v>
+      </c>
+      <c r="J13" s="11">
+        <v>2</v>
+      </c>
+      <c r="K13" s="11">
+        <v>2</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A15" s="2">
+        <v>11</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="A16" s="2">
+        <v>12</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A20" s="2">
+        <v>16</v>
+      </c>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A22" s="2">
+        <v>18</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A23" s="2">
+        <v>19</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A24" s="2">
+        <v>20</v>
+      </c>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A25" s="2">
+        <v>21</v>
+      </c>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A26" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A27" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A28" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A29" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A30" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A31" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
- NEW nlconv.py for ADC2017
</commit_message>
<xml_diff>
--- a/support/sample.xlsx
+++ b/support/sample.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="23580" windowHeight="11250" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="23580" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Q4.1" sheetId="4" r:id="rId4"/>
     <sheet name="Q4.2" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -426,12 +426,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -473,7 +476,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -508,7 +511,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -719,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -4568,7 +4571,7 @@
   <dimension ref="A1:AK39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5544,8 +5547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>